<commit_message>
Add ActiveSheet property (Issue #10)
</commit_message>
<xml_diff>
--- a/Assets/Development/TestFiles/FiveSheets.xlsx
+++ b/Assets/Development/TestFiles/FiveSheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APLProjects\CarlisleGroup\XL2APL\Assets\Development\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APLProjects\XL2APL\Assets\Development\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E56F4D-63BF-4261-9329-A7B746961824}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB34D05-D7C4-4688-8281-E6DFBC567ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{A9437C1A-FDF2-4050-A3FA-83E6FD2440E8}"/>
+    <workbookView xWindow="-28800" yWindow="-12570" windowWidth="28830" windowHeight="15630" activeTab="4" xr2:uid="{A9437C1A-FDF2-4050-A3FA-83E6FD2440E8}"/>
   </bookViews>
   <sheets>
     <sheet name="One" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE357E0-D9A9-4B8C-9F20-0797F78C0054}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -535,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8463F1AD-0FB7-41CC-BEB0-D38E60BDCC95}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>